<commit_message>
feat: refactor register-user-information exception and error handling
</commit_message>
<xml_diff>
--- a/archivos/TestRegistroEstudiantes.xlsx
+++ b/archivos/TestRegistroEstudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Desktop/Universidad/Proyecto Integrador/PI1/icesi-filantrop-a-equipo-2/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B78882B-4CB5-2944-97D3-812F24B70CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D186B-BD8B-024A-BD86-2CB993B933A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="2180" windowWidth="17480" windowHeight="14960" xr2:uid="{4AB53052-041A-554A-90C9-48D2A5716275}"/>
+    <workbookView xWindow="13920" yWindow="3280" windowWidth="17480" windowHeight="14960" xr2:uid="{4AB53052-041A-554A-90C9-48D2A5716275}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>tipo_documento</t>
   </si>
@@ -86,12 +86,6 @@
     <t>jperez@institucion.edu</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>Masculino</t>
-  </si>
-  <si>
     <t>TI</t>
   </si>
   <si>
@@ -104,12 +98,6 @@
     <t>mrodriguez@institucion.edu</t>
   </si>
   <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
     <t>MR002</t>
   </si>
   <si>
@@ -125,12 +113,6 @@
     <t>jdoe@institucion.edu</t>
   </si>
   <si>
-    <t>4.8</t>
-  </si>
-  <si>
-    <t>Otro</t>
-  </si>
-  <si>
     <t>JD003</t>
   </si>
   <si>
@@ -143,106 +125,22 @@
     <t>pgomez@institucion.edu</t>
   </si>
   <si>
-    <t>4.6</t>
-  </si>
-  <si>
     <t>PG004</t>
   </si>
   <si>
-    <t>CE</t>
-  </si>
-  <si>
-    <t>Luisa Fernandez</t>
-  </si>
-  <si>
-    <t>lfernandez@gmail.com</t>
-  </si>
-  <si>
-    <t>lfernandez@institucion.edu</t>
-  </si>
-  <si>
-    <t>4.7</t>
-  </si>
-  <si>
-    <t>LN005</t>
-  </si>
-  <si>
-    <t>Jorge Martinez</t>
-  </si>
-  <si>
-    <t>jmartinez@gmail.com</t>
-  </si>
-  <si>
-    <t>jmartinez@institucion.edu</t>
-  </si>
-  <si>
-    <t>JM006</t>
-  </si>
-  <si>
-    <t>RC</t>
-  </si>
-  <si>
-    <t>Sofia Torres</t>
-  </si>
-  <si>
-    <t>storrres@gmail.com</t>
-  </si>
-  <si>
-    <t>storrres@institucion.edu</t>
-  </si>
-  <si>
-    <t>4.9</t>
-  </si>
-  <si>
-    <t>SF007</t>
-  </si>
-  <si>
-    <t>Laura Ramirez</t>
-  </si>
-  <si>
-    <t>lramirez@gmail.com</t>
-  </si>
-  <si>
-    <t>lramirez@institucion.edu</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>LZ008</t>
-  </si>
-  <si>
-    <t>Daniel Morales</t>
-  </si>
-  <si>
-    <t>dmorales@gmail.com</t>
-  </si>
-  <si>
-    <t>dmorales@institucion.edu</t>
-  </si>
-  <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>Camila Sanchez</t>
-  </si>
-  <si>
-    <t>casanchez@gmail.com</t>
-  </si>
-  <si>
-    <t>casanchez@institucion.edu</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
     <t>A00156800</t>
   </si>
   <si>
-    <t>A00492300</t>
-  </si>
-  <si>
-    <t>A00123920</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>5.0</t>
   </si>
 </sst>
 </file>
@@ -596,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFC6B80-1155-874F-8590-F55FA02751BB}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="F2">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="G2" s="2">
         <v>36526</v>
@@ -682,36 +580,36 @@
         <v>3001234567</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="J2">
         <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>987654321</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F3">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="G3" s="2">
         <v>36924</v>
@@ -720,33 +618,33 @@
         <v>3009876543</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="J3">
         <v>110</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>212345678</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>500</v>
@@ -758,16 +656,16 @@
         <v>3001357924</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J4">
         <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -778,16 +676,16 @@
         <v>2345678901</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="G5" s="2">
         <v>37715</v>
@@ -796,244 +694,16 @@
         <v>3002468135</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5">
         <v>140</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>123456789</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <v>470</v>
-      </c>
-      <c r="G6" s="2">
-        <v>38112</v>
-      </c>
-      <c r="H6">
-        <v>3003579246</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6">
-        <v>150</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>3456789012</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7">
-        <v>480</v>
-      </c>
-      <c r="G7" s="2">
-        <v>38509</v>
-      </c>
-      <c r="H7">
-        <v>3004681357</v>
-      </c>
-      <c r="I7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7">
-        <v>160</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8">
-        <v>534567890</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8">
-        <v>490</v>
-      </c>
-      <c r="G8" s="2">
-        <v>38905</v>
-      </c>
-      <c r="H8">
-        <v>3005792468</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8">
-        <v>170</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>8456789012</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9">
-        <v>430</v>
-      </c>
-      <c r="G9" s="2">
-        <v>39302</v>
-      </c>
-      <c r="H9">
-        <v>3006897579</v>
-      </c>
-      <c r="I9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9">
-        <v>90</v>
-      </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>9567890123</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10">
-        <v>310</v>
-      </c>
-      <c r="G10" s="2">
-        <v>39700</v>
-      </c>
-      <c r="H10">
-        <v>3008004190</v>
-      </c>
-      <c r="I10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10">
-        <v>80</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
-        <v>11678901234</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11">
-        <v>300</v>
-      </c>
-      <c r="G11" s="2">
-        <v>40096</v>
-      </c>
-      <c r="H11">
-        <v>3009110801</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11">
-        <v>70</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: refactor update-user-information with excel file and HTML form
</commit_message>
<xml_diff>
--- a/archivos/TestRegistroEstudiantes.xlsx
+++ b/archivos/TestRegistroEstudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Desktop/Universidad/Proyecto Integrador/PI1/icesi-filantrop-a-equipo-2/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D186B-BD8B-024A-BD86-2CB993B933A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AACAD22-E79F-C149-B7A7-D0E76FA4EBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13920" yWindow="3280" windowWidth="17480" windowHeight="14960" xr2:uid="{4AB53052-041A-554A-90C9-48D2A5716275}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>tipo_documento</t>
   </si>
@@ -86,9 +86,6 @@
     <t>jperez@institucion.edu</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>Maria Rodriguez</t>
   </si>
   <si>
@@ -141,16 +138,42 @@
   </si>
   <si>
     <t>5.0</t>
+  </si>
+  <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>andres@gmail.com</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>A00123300</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>3.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,15 +196,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFC6B80-1155-874F-8590-F55FA02751BB}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +597,7 @@
         <v>15</v>
       </c>
       <c r="F2">
-        <v>500</v>
+        <v>409</v>
       </c>
       <c r="G2" s="2">
         <v>36526</v>
@@ -580,36 +606,36 @@
         <v>3001234567</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="J2">
         <v>120</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>987654321</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F3">
-        <v>500</v>
+        <v>123</v>
       </c>
       <c r="G3" s="2">
         <v>36924</v>
@@ -618,36 +644,36 @@
         <v>3009876543</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3">
         <v>110</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>212345678</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F4">
-        <v>500</v>
+        <v>390</v>
       </c>
       <c r="G4" s="2">
         <v>37318</v>
@@ -656,16 +682,16 @@
         <v>3001357924</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J4">
         <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -676,16 +702,16 @@
         <v>2345678901</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F5">
-        <v>500</v>
+        <v>123</v>
       </c>
       <c r="G5" s="2">
         <v>37715</v>
@@ -694,19 +720,61 @@
         <v>3002468135</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>140</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1107834925</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>320</v>
+      </c>
+      <c r="G6" s="2">
+        <v>38054</v>
+      </c>
+      <c r="H6">
+        <v>3207282500</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{6F4A4FBA-2EE0-5F47-B7A2-CD02BE7FFB52}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{435DF618-2A8D-9A44-848F-33D9E1000EF5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>